<commit_message>
Several changes to classes and list of cells
</commit_message>
<xml_diff>
--- a/datafiles/how.xlsx
+++ b/datafiles/how.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\workspace eclipse\POIApache\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DE9833-933B-4900-B37F-D1EAE89171C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01DB982-3CD3-4075-B204-9D819812C02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,40 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Colum 1 - Row 1</t>
-  </si>
-  <si>
-    <t>Column 2 - Row 1</t>
-  </si>
-  <si>
-    <t>Column 3 - Row 1</t>
-  </si>
-  <si>
-    <t>Colum 1 - Row 2</t>
-  </si>
-  <si>
-    <t>Colum 1 - Row 3</t>
-  </si>
-  <si>
-    <t>Column 2 - Row 2</t>
-  </si>
-  <si>
-    <t>Column 2 - Row 3</t>
-  </si>
-  <si>
-    <t>Column 3 - Row 2</t>
-  </si>
-  <si>
-    <t>Column 3 - Row 3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>Lorena</t>
+  </si>
+  <si>
+    <t>Brazil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,16 +63,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,12 +94,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,7 +407,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,39 +418,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented successful list comparison with hashset
</commit_message>
<xml_diff>
--- a/datafiles/how.xlsx
+++ b/datafiles/how.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\workspace eclipse\POIApache\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01DB982-3CD3-4075-B204-9D819812C02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFBA38B-F629-43FF-B0A5-1816BF79FFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,37 +25,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>Mother</t>
-  </si>
-  <si>
-    <t>Son</t>
-  </si>
-  <si>
-    <t>Lorena</t>
-  </si>
-  <si>
-    <t>Brazil</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>WDPE059A50</t>
+  </si>
+  <si>
+    <t>WDPE059A51</t>
+  </si>
+  <si>
+    <t>WDPE059A52</t>
+  </si>
+  <si>
+    <t>WDPE059A53</t>
+  </si>
+  <si>
+    <t>WDPE059A54</t>
+  </si>
+  <si>
+    <t>WDPE059A55</t>
+  </si>
+  <si>
+    <t>WDPE059A56</t>
+  </si>
+  <si>
+    <t>WDPE059A57</t>
+  </si>
+  <si>
+    <t>WDPE059A58</t>
+  </si>
+  <si>
+    <t>WDPE059A59</t>
+  </si>
+  <si>
+    <t>WDPE059A60</t>
+  </si>
+  <si>
+    <t>WDPE059A61</t>
+  </si>
+  <si>
+    <t>WDPE059A62</t>
+  </si>
+  <si>
+    <t>WDPE059A63</t>
+  </si>
+  <si>
+    <t>WDPE059A64</t>
+  </si>
+  <si>
+    <t>WDPE059A65</t>
+  </si>
+  <si>
+    <t>WDPE059A66</t>
+  </si>
+  <si>
+    <t>WDPE059A67</t>
+  </si>
+  <si>
+    <t>WDPE059A68</t>
+  </si>
+  <si>
+    <t>WDPE059A69</t>
+  </si>
+  <si>
+    <t>WDPE059A70</t>
+  </si>
+  <si>
+    <t>WDPE059A71</t>
+  </si>
+  <si>
+    <t>WDPE059A72</t>
+  </si>
+  <si>
+    <t>WDPE059A73</t>
+  </si>
+  <si>
+    <t>WDPE059A74</t>
+  </si>
+  <si>
+    <t>WDPE059A75</t>
+  </si>
+  <si>
+    <t>WDPE059A76</t>
+  </si>
+  <si>
+    <t>WDPE059A77</t>
+  </si>
+  <si>
+    <t>WDPE059A78</t>
+  </si>
+  <si>
+    <t>WDPE059A79</t>
+  </si>
+  <si>
+    <t>WDPE059A80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +139,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,11 +191,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -404,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,40 +492,168 @@
     <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>